<commit_message>
Fixed lab work 9,10
</commit_message>
<xml_diff>
--- a/lab-9,10/lab9,10.xlsx
+++ b/lab-9,10/lab9,10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-план" sheetId="1" r:id="rId1"/>
@@ -857,6 +857,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,6 +870,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -886,13 +893,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2695,8 +2695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2709,12 +2709,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="3" spans="3:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
@@ -2722,20 +2722,20 @@
       </c>
     </row>
     <row r="4" spans="3:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="6" spans="3:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="8" spans="3:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
@@ -2764,7 +2764,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
@@ -2876,10 +2876,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -3117,10 +3117,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -3268,10 +3268,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -3439,10 +3439,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -3628,10 +3628,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -3779,10 +3779,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -4028,7 +4028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -4039,11 +4039,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:6" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="4:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D2" s="1" t="s">
@@ -4067,10 +4067,10 @@
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="47"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="5" spans="4:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D5" s="1"/>
@@ -4132,67 +4132,67 @@
       <c r="D11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="55">
         <v>4</v>
       </c>
-      <c r="F11" s="53"/>
+      <c r="F11" s="56"/>
     </row>
     <row r="12" spans="4:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="57">
         <v>0</v>
       </c>
-      <c r="F12" s="55"/>
+      <c r="F12" s="58"/>
     </row>
     <row r="13" spans="4:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D13" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="57">
         <v>0</v>
       </c>
-      <c r="F13" s="55"/>
+      <c r="F13" s="58"/>
     </row>
     <row r="14" spans="4:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="57">
         <v>3</v>
       </c>
-      <c r="F14" s="55"/>
+      <c r="F14" s="58"/>
     </row>
     <row r="15" spans="4:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="D15" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="57">
         <v>1</v>
       </c>
-      <c r="F15" s="55"/>
+      <c r="F15" s="58"/>
     </row>
     <row r="16" spans="4:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="50">
+      <c r="E16" s="53">
         <v>0</v>
       </c>
-      <c r="F16" s="51"/>
+      <c r="F16" s="54"/>
     </row>
     <row r="18" spans="4:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="46" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="19" spans="4:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>